<commit_message>
Updated STLs and some gantry work
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Item</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>http://www.amazon.com/RepRap-Aluminum-Timing-Pulley-Printer/dp/B00GNWMTWG/ref=sr_1_3?ie=UTF8&amp;qid=1411877142&amp;sr=8-3&amp;keywords=gt2+pulley</t>
+  </si>
+  <si>
+    <t>GT2 Belt</t>
+  </si>
+  <si>
+    <t>Linear Motion 8 mm Shaft</t>
   </si>
 </sst>
 </file>
@@ -139,8 +145,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E5" totalsRowShown="0">
-  <autoFilter ref="A2:E5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E7" totalsRowShown="0">
+  <autoFilter ref="A2:E7"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Item"/>
     <tableColumn id="2" name="quantity"/>
@@ -417,13 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.90625" customWidth="1"/>
     <col min="5" max="5" width="127.90625" bestFit="1" customWidth="1"/>
   </cols>
@@ -506,6 +514,26 @@
       </c>
       <c r="E5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <f>Table1[quantity]*Table1[price]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
+        <f>Table1[quantity]*Table1[price]</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gantry belt lock update
Gantry belt lock was added, still needs clamps and tensioner. pulleys
were added to bom.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="940" yWindow="0" windowWidth="13680" windowHeight="5580"/>
+    <workbookView xWindow="1880" yWindow="0" windowWidth="13680" windowHeight="5580"/>
   </bookViews>
   <sheets>
     <sheet name="Simple BOM" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Item</t>
   </si>
@@ -56,16 +56,22 @@
     <t>http://www.amazon.com/VXB-Skateboard-Bearings-Double-Shielded/dp/B002BBGTK6/ref=sr_1_6?ie=UTF8&amp;qid=1411876962&amp;sr=8-6&amp;keywords=608</t>
   </si>
   <si>
-    <t>GT2 pulley</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/RepRap-Aluminum-Timing-Pulley-Printer/dp/B00GNWMTWG/ref=sr_1_3?ie=UTF8&amp;qid=1411877142&amp;sr=8-3&amp;keywords=gt2+pulley</t>
-  </si>
-  <si>
     <t>GT2 Belt</t>
   </si>
   <si>
     <t>Linear Motion 8 mm Shaft</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/RepRap-Aluminum-Timing-Pulley-Printer/dp/B00GNWQL48/ref=sr_1_2?ie=UTF8&amp;qid=1412055779&amp;sr=8-2&amp;keywords=gt2+8mm+bore</t>
+  </si>
+  <si>
+    <t>GT2 pulley (Shafts)</t>
+  </si>
+  <si>
+    <t>GT2 Pulley (motor)</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/RepRap-Aluminum-Timing-Pulley-Printer/dp/B00GNWMTWG/ref=sr_1_3?ie=UTF8&amp;qid=1412056034&amp;sr=8-3&amp;keywords=gt2+5mm+bore</t>
   </si>
 </sst>
 </file>
@@ -145,8 +151,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E7" totalsRowShown="0">
-  <autoFilter ref="A2:E7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E8" totalsRowShown="0">
+  <autoFilter ref="A2:E8"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Item"/>
     <tableColumn id="2" name="quantity"/>
@@ -423,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -442,7 +448,7 @@
       </c>
       <c r="D1">
         <f>SUM(Table1[sub Tot])</f>
-        <v>66.400000000000006</v>
+        <v>89.6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -500,38 +506,56 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
         <v>10</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
       </c>
       <c r="C5" s="2">
         <v>5.8</v>
       </c>
       <c r="D5" s="2">
         <f>Table1[quantity]*Table1[price]</f>
-        <v>46.4</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5.8</v>
+      </c>
       <c r="D6" s="2">
         <f>Table1[quantity]*Table1[price]</f>
-        <v>0</v>
+        <v>11.6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2">
+        <f>Table1[quantity]*Table1[price]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
         <f>Table1[quantity]*Table1[price]</f>
         <v>0</v>
       </c>

</xml_diff>